<commit_message>
Add Attack Message & Sqlite DB *Not connect yet
</commit_message>
<xml_diff>
--- a/Mapping.xlsx
+++ b/Mapping.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D39A21-B282-436D-B71D-8F95F24EFFB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3078AE87-C56E-453B-93CD-8F6035CD3C84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1297,13 +1297,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3B87916-FCAD-4CB0-BBD2-BB3EFD8B9556}" name="表格1" displayName="表格1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
-  <autoFilter ref="A1:H26" xr:uid="{D201716D-6079-4CED-B8AC-4098AAC121C4}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Character"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H26" xr:uid="{D201716D-6079-4CED-B8AC-4098AAC121C4}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{21D88FD5-E2DA-4C31-8938-FD4CA3CB8963}" name="Entity Name" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{9A2F97F8-FC34-4D84-A5EC-97C45EC0C684}" name="Entity Definition" dataDxfId="22"/>
@@ -1619,7 +1613,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,7 +1655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -1687,7 +1681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
@@ -1711,7 +1705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1733,7 +1727,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -1755,7 +1749,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -2211,7 +2205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>41</v>
       </c>
@@ -2237,7 +2231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Add Room Entity and rebuild folder location
</commit_message>
<xml_diff>
--- a/Mapping.xlsx
+++ b/Mapping.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3078AE87-C56E-453B-93CD-8F6035CD3C84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B98B0C-F5AA-4349-8636-D53E296E8AAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
     <sheet name="Monster" sheetId="2" r:id="rId2"/>
-    <sheet name="Rooms" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups" sheetId="4" r:id="rId3"/>
+    <sheet name="Rooms" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="113">
   <si>
     <t>Entity Name</t>
   </si>
@@ -324,6 +325,150 @@
   <si>
     <t>Account Money</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ch_Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mns_Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room Detail</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ro_Dtl</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ro_No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ch_No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mns_No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ro_Nm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ro_Type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room Type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ro_Bos_No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room Boss Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre_Ro_No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PreRoom Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Child_Ro_No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Child Room Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ro_Lv</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room Level</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mns_Group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster Group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mns_Grp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mns_Grp_No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster Group Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room Route</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ro_Rou</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -369,7 +514,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,44 +527,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -533,60 +653,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="54">
     <dxf>
       <font>
         <b/>
@@ -611,6 +733,819 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -891,6 +1826,44 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1296,51 +2269,71 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3B87916-FCAD-4CB0-BBD2-BB3EFD8B9556}" name="表格1" displayName="表格1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
-  <autoFilter ref="A1:H26" xr:uid="{D201716D-6079-4CED-B8AC-4098AAC121C4}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{21D88FD5-E2DA-4C31-8938-FD4CA3CB8963}" name="Entity Name" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{9A2F97F8-FC34-4D84-A5EC-97C45EC0C684}" name="Entity Definition" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{68C7B960-EEE7-4168-8CF6-552CAD97F5C6}" name="Table Name" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{29BC5DD7-5634-4399-AF0E-98D2729DA983}" name="Column Name" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{54F27F78-4F6D-4FAB-A0B5-DF72ABB86E79}" name="Attribute Name" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{3CCA3898-1AF9-47F7-8D8B-718A7C456D27}" name="Column Datatype" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{98AC24BD-7BBF-4114-A5D4-9382602A35F5}" name="PK" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{DE2305E8-878C-4593-8C2E-F39F69E557F4}" name="Required" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3B87916-FCAD-4CB0-BBD2-BB3EFD8B9556}" name="表格1" displayName="表格1" ref="A1:I27" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+  <autoFilter ref="A1:I27" xr:uid="{D201716D-6079-4CED-B8AC-4098AAC121C4}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{21D88FD5-E2DA-4C31-8938-FD4CA3CB8963}" name="Entity Name" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{9A2F97F8-FC34-4D84-A5EC-97C45EC0C684}" name="Entity Definition" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{68C7B960-EEE7-4168-8CF6-552CAD97F5C6}" name="Table Name" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{29BC5DD7-5634-4399-AF0E-98D2729DA983}" name="Column Name" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{54F27F78-4F6D-4FAB-A0B5-DF72ABB86E79}" name="Attribute Name" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{3CCA3898-1AF9-47F7-8D8B-718A7C456D27}" name="Column Datatype" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{98AC24BD-7BBF-4114-A5D4-9382602A35F5}" name="PK" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{DE2305E8-878C-4593-8C2E-F39F69E557F4}" name="Required" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{3F87F2B0-13EA-4F59-A028-553A1093774F}" name="Remark" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E536EA4B-000D-47F1-8586-203B763AFEA9}" name="表格2" displayName="表格2" ref="A1:H14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:H14" xr:uid="{C0C7D80C-4D57-44F0-AED1-56E0C9E3DCFE}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{EFBB6266-9042-4FD0-B5D2-C6711C771A14}" name="Entity Name" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{68E6B300-D3DC-485D-8A3C-0B4061AE30F5}" name="Entity Definition" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{4F443399-6DAB-4A6F-B2D9-E65110EB5876}" name="Table Name" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{5B2D5538-6175-49D5-B260-0636D07B02B6}" name="Column Name" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{1E3BE83F-62CE-4290-8BB8-61CE210A09B5}" name="Attribute Name" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{1F771DBE-DF22-4F5D-B820-D9EA588944DB}" name="Column Datatype" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{9602F387-B445-44E8-A122-2CFDF4AFDE2F}" name="PK" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{A2B36E5A-2E55-42F2-A5EB-B6F95FA7D368}" name="Required" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E536EA4B-000D-47F1-8586-203B763AFEA9}" name="表格2" displayName="表格2" ref="A1:I15" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+  <autoFilter ref="A1:I15" xr:uid="{C0C7D80C-4D57-44F0-AED1-56E0C9E3DCFE}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{EFBB6266-9042-4FD0-B5D2-C6711C771A14}" name="Entity Name" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{68E6B300-D3DC-485D-8A3C-0B4061AE30F5}" name="Entity Definition" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{4F443399-6DAB-4A6F-B2D9-E65110EB5876}" name="Table Name" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{5B2D5538-6175-49D5-B260-0636D07B02B6}" name="Column Name" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{1E3BE83F-62CE-4290-8BB8-61CE210A09B5}" name="Attribute Name" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{1F771DBE-DF22-4F5D-B820-D9EA588944DB}" name="Column Datatype" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{9602F387-B445-44E8-A122-2CFDF4AFDE2F}" name="PK" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{A2B36E5A-2E55-42F2-A5EB-B6F95FA7D368}" name="Required" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{DAAA8CEF-6B52-46DB-8D5E-30227C50B62B}" name="Remark" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7DBA1A15-6620-45E6-AFD8-206BC5F80656}" name="表格4" displayName="表格4" ref="A1:H4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:H4" xr:uid="{D20A76BD-34B2-43F2-8246-CFC3E4D1E081}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CAD6D4F8-8FB9-46FA-900C-22073001F94E}" name="表格3" displayName="表格3" ref="A1:I3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="21" headerRowBorderDxfId="23" tableBorderDxfId="24">
+  <autoFilter ref="A1:I3" xr:uid="{DDDD9532-CFA9-4E22-B0AF-4875CCF9FDD0}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{9A7300B6-D49C-42B9-9726-3327A5395FC6}" name="Entity Name" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{D95DCCB4-A2CC-4EFC-8CAC-E023860F10F9}" name="Entity Definition" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{2581AED9-7AE7-404A-8EE0-853246B557A9}" name="Table Name" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{A5A7E079-D8F4-4207-AE15-921AED7422CA}" name="Column Name" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{7518393A-279E-4CA6-84E0-CDCA6A1376A9}" name="Attribute Name" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{ED147885-CDB3-4946-9821-E83082CA21FA}" name="Column Datatype" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{4B6980A6-49C1-4AC1-B428-5A44001CA66A}" name="PK" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{1DE86D00-6E02-4495-99E2-F14A858C551C}" name="Required" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{52A811D1-7E0D-4BFD-94CA-B6046B64BAD9}" name="Remark" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7DBA1A15-6620-45E6-AFD8-206BC5F80656}" name="表格4" displayName="表格4" ref="A1:H11" totalsRowShown="0" headerRowDxfId="0" dataDxfId="25" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:H11" xr:uid="{D20A76BD-34B2-43F2-8246-CFC3E4D1E081}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{84A56582-B701-47EC-81D9-A79364D31EDF}" name="Entity Name"/>
-    <tableColumn id="2" xr3:uid="{CECB7E08-04AD-4630-B3DE-8502FEA16E63}" name="Entity Definition"/>
-    <tableColumn id="3" xr3:uid="{0C65E5D8-5A91-4D01-8C01-E374DF43F1BB}" name="Table Name"/>
-    <tableColumn id="4" xr3:uid="{996CCCA4-16B1-4CDF-B710-A2A6BFAB0D93}" name="Column Name"/>
-    <tableColumn id="5" xr3:uid="{E457B014-E655-4A39-9311-AEFBF7F7568C}" name="Attribute Name"/>
-    <tableColumn id="6" xr3:uid="{394C1BDE-1C26-4A45-B0DE-2C839963F912}" name="Column Datatype"/>
-    <tableColumn id="7" xr3:uid="{B6177833-3216-4495-BF75-01B8F9D2D4BE}" name="PK"/>
-    <tableColumn id="8" xr3:uid="{5DDE3391-78F2-44EF-95E8-4968F9326662}" name="Required"/>
+    <tableColumn id="1" xr3:uid="{84A56582-B701-47EC-81D9-A79364D31EDF}" name="Entity Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{CECB7E08-04AD-4630-B3DE-8502FEA16E63}" name="Entity Definition" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0C65E5D8-5A91-4D01-8C01-E374DF43F1BB}" name="Table Name" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{996CCCA4-16B1-4CDF-B710-A2A6BFAB0D93}" name="Column Name" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{E457B014-E655-4A39-9311-AEFBF7F7568C}" name="Attribute Name" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{394C1BDE-1C26-4A45-B0DE-2C839963F912}" name="Column Datatype" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{B6177833-3216-4495-BF75-01B8F9D2D4BE}" name="PK" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{5DDE3391-78F2-44EF-95E8-4968F9326662}" name="Required" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1609,11 +2602,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,634 +2619,690 @@
     <col min="6" max="6" width="19.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="I1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="G7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="7">
+        <v>20201208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D15" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="G15" s="7"/>
+      <c r="H15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="G16" s="7"/>
+      <c r="H16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="G17" s="7"/>
+      <c r="H17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="G18" s="7"/>
+      <c r="H18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="G19" s="7"/>
+      <c r="H19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D20" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="G20" s="7"/>
+      <c r="H20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D21" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="G21" s="7"/>
+      <c r="H21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D22" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="G22" s="7"/>
+      <c r="H22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D23" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F23" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B24" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D24" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="G24" s="7"/>
+      <c r="H24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D25" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F25" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="G25" s="7"/>
+      <c r="H25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D26" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E26" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="G26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B27" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C27" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D27" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E27" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2266,10 +3315,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D0A7CB-ED19-4588-B0DD-C504FD6D67DF}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,348 +3331,392 @@
     <col min="6" max="6" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="I1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="G2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="7">
+        <v>20201208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2635,11 +3728,140 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89EA31-7143-43F0-8F61-0BDD0B3E8F2D}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A039DA74-464C-4564-9F37-3CC52BEAF785}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2655,36 +3877,279 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="18" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>